<commit_message>
leaps and bounds or something
</commit_message>
<xml_diff>
--- a/projectJournal.xlsx
+++ b/projectJournal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmyMi\Documents\College\psychic-memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170FBAAB-78FA-4C54-BA5C-42AC67F0C975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8E5A2B-01D9-47FC-B9F2-8B84E3B072CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{F17A8DAE-DCCF-4D99-88A2-688B9328FBFC}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12585" xr2:uid="{F17A8DAE-DCCF-4D99-88A2-688B9328FBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -142,13 +142,22 @@
     <t>Monday 18 April 2022</t>
   </si>
   <si>
-    <t>13:00-23:00</t>
-  </si>
-  <si>
-    <t>Major bugfixing and save functionality.</t>
-  </si>
-  <si>
     <t>Base world system.</t>
+  </si>
+  <si>
+    <t>13:00-24:00</t>
+  </si>
+  <si>
+    <t>Options functionality and persistant data.</t>
+  </si>
+  <si>
+    <t>Tuesday 19 April 2022</t>
+  </si>
+  <si>
+    <t>03:30-05:00</t>
+  </si>
+  <si>
+    <t>Save and high score system.</t>
   </si>
 </sst>
 </file>
@@ -653,11 +662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C6DC7B-4D2D-451F-89A0-A814AEACCE79}">
-  <dimension ref="B1:F12"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB14" sqref="AB14"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +759,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -860,16 +869,33 @@
         <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scrolling background and functional save file again
</commit_message>
<xml_diff>
--- a/projectJournal.xlsx
+++ b/projectJournal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmyMi\Documents\College\psychic-memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CA93B4-C1B1-40D5-AC77-EEA9F8E5779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63592253-792D-41D5-9CF7-BA83AA3C4A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12585" xr2:uid="{F17A8DAE-DCCF-4D99-88A2-688B9328FBFC}"/>
   </bookViews>
@@ -178,10 +178,10 @@
     <t>Friday 22 April 2022</t>
   </si>
   <si>
-    <t>17:00-03:00</t>
-  </si>
-  <si>
     <t>Level polish and Documentation.</t>
+  </si>
+  <si>
+    <t>17:00-06:00</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,13 +916,13 @@
         <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="9">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D17" s="9">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>